<commit_message>
Flash success on upload works
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Chile</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>region</t>
+  </si>
+  <si>
+    <t>China</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -451,6 +454,14 @@
       </c>
       <c r="B5">
         <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data updated to 23 countries and Sansus font on all site.
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Chile</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>Italy</t>
   </si>
   <si>
@@ -40,6 +37,63 @@
   </si>
   <si>
     <t>China</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>ANZ</t>
+  </si>
+  <si>
+    <t>Benelux</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Iberia</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Saudi</t>
+  </si>
+  <si>
+    <t>Gulf</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>S Africa</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Russia</t>
   </si>
 </sst>
 </file>
@@ -63,9 +117,29 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -75,8 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,60 +484,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B5">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
         <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data update for circle fills targeting
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Chile</t>
   </si>
@@ -96,17 +96,42 @@
     <t>Russia</t>
   </si>
   <si>
-    <t>Image</t>
+    <t>circle1</t>
+  </si>
+  <si>
+    <t>circle2</t>
+  </si>
+  <si>
+    <t>circle3</t>
+  </si>
+  <si>
+    <t>circle4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,15 +174,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,15 +544,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -505,262 +562,479 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>99</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>80</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7">
         <v>20</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <v>40</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <v>50</v>
       </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B10">
         <v>30</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>50</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13">
         <v>60</v>
       </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B14">
         <v>40</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16">
         <v>50</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B17">
         <v>10</v>
       </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B18">
         <v>60</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B19">
         <v>44</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>22</v>
       </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>66</v>
       </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>77</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>44</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
-      <c r="C24">
-        <v>3</v>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Sort fix, decent demonstration version
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -114,9 +114,6 @@
     <t>jp</t>
   </si>
   <si>
-    <t>uk</t>
-  </si>
-  <si>
     <t>de</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>kr</t>
+  </si>
+  <si>
+    <t>gb</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -641,7 +641,7 @@
         <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -649,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -695,7 +695,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -741,7 +741,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -764,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -787,7 +787,7 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -802,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -810,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -856,7 +856,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -879,7 +879,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -902,7 +902,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -925,7 +925,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -971,22 +971,22 @@
         <v>17</v>
       </c>
       <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -994,7 +994,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1017,7 +1017,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1060,7 +1060,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1075,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1083,7 +1083,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1106,7 +1106,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1121,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1129,7 +1129,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1152,7 +1152,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
@@ -1167,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flags in ui-grid working, added UAE flag
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Chile</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>gb</t>
+  </si>
+  <si>
+    <t>ae</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1030,6 +1033,9 @@
       </c>
       <c r="F18" t="b">
         <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:7">

</xml_diff>